<commit_message>
Add some more outputs and observations
</commit_message>
<xml_diff>
--- a/Tests/Validation/Maize/Observations/MaizeObservations.xlsx
+++ b/Tests/Validation/Maize/Observations/MaizeObservations.xlsx
@@ -15,7 +15,7 @@
     <sheet name="Observed" sheetId="1" r:id="rId1"/>
   </sheets>
   <definedNames>
-    <definedName name="_xlnm._FilterDatabase" localSheetId="0" hidden="1">Observed!$A$1:$A$1633</definedName>
+    <definedName name="_xlnm._FilterDatabase" localSheetId="0" hidden="1">Observed!$A$1:$AJ$1633</definedName>
   </definedNames>
   <calcPr calcId="152511"/>
 </workbook>
@@ -806,12 +806,15 @@
   <cellStyleXfs count="1">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
   </cellStyleXfs>
-  <cellXfs count="3">
+  <cellXfs count="4">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="0" fontId="1" fillId="0" borderId="1" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="top"/>
     </xf>
     <xf numFmtId="164" fontId="1" fillId="0" borderId="1" xfId="0" applyNumberFormat="1" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="top"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyNumberFormat="1" applyAlignment="1">
       <alignment horizontal="center" vertical="top"/>
     </xf>
   </cellXfs>
@@ -1121,10 +1124,10 @@
   <dimension ref="A1:BQ1633"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
-      <pane xSplit="2" ySplit="1" topLeftCell="C2" activePane="bottomRight" state="frozen"/>
+      <pane xSplit="2" ySplit="1" topLeftCell="E75" activePane="bottomRight" state="frozen"/>
       <selection pane="topRight" activeCell="C1" sqref="C1"/>
       <selection pane="bottomLeft" activeCell="A2" sqref="A2"/>
-      <selection pane="bottomRight" sqref="A1:BQ1633"/>
+      <selection pane="bottomRight" activeCell="G1281" sqref="G1281"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -3425,6 +3428,9 @@
       <c r="D74">
         <v>2020.8</v>
       </c>
+      <c r="H74" s="3">
+        <v>98.4</v>
+      </c>
       <c r="K74">
         <v>4872.3193140000003</v>
       </c>
@@ -3511,6 +3517,13 @@
       <c r="D75">
         <v>767.7</v>
       </c>
+      <c r="G75">
+        <f>H75*U75</f>
+        <v>0.67858379999999996</v>
+      </c>
+      <c r="H75" s="3">
+        <v>111.6</v>
+      </c>
       <c r="K75">
         <v>2053.284181</v>
       </c>
@@ -3594,6 +3607,13 @@
       <c r="D76">
         <v>2442.6999999999998</v>
       </c>
+      <c r="G76">
+        <f>H76*U76</f>
+        <v>0.74290499999999982</v>
+      </c>
+      <c r="H76" s="3">
+        <v>89.999999999999986</v>
+      </c>
       <c r="K76">
         <v>5012.0274069999996</v>
       </c>
@@ -3677,6 +3697,13 @@
       <c r="D77">
         <v>1105.0999999999999</v>
       </c>
+      <c r="G77">
+        <f>H77*U77</f>
+        <v>1.016821</v>
+      </c>
+      <c r="H77" s="3">
+        <v>139.1</v>
+      </c>
       <c r="K77">
         <v>2666.9280370000001</v>
       </c>
@@ -3760,6 +3787,13 @@
       <c r="D78">
         <v>2833.9</v>
       </c>
+      <c r="G78">
+        <f>H78*U78</f>
+        <v>1.898053625</v>
+      </c>
+      <c r="H78" s="3">
+        <v>188.5</v>
+      </c>
       <c r="K78">
         <v>5640.0645649999997</v>
       </c>
@@ -3843,6 +3877,13 @@
       <c r="D79">
         <v>1192.8</v>
       </c>
+      <c r="G79">
+        <f>H79*U79</f>
+        <v>1.1876796000000001</v>
+      </c>
+      <c r="H79" s="3">
+        <v>155.69999999999999</v>
+      </c>
       <c r="K79">
         <v>2965.1934860000001</v>
       </c>
@@ -20739,6 +20780,13 @@
       <c r="D1051">
         <v>53.3</v>
       </c>
+      <c r="G1051">
+        <f>H1051*U1051</f>
+        <v>0</v>
+      </c>
+      <c r="H1051" s="3">
+        <v>0</v>
+      </c>
       <c r="M1051">
         <v>0</v>
       </c>
@@ -21228,6 +21276,13 @@
       <c r="D1066">
         <v>841.9</v>
       </c>
+      <c r="G1066">
+        <f>H1066*U1066</f>
+        <v>9.7554700000000008E-2</v>
+      </c>
+      <c r="H1066" s="3">
+        <v>17.3</v>
+      </c>
       <c r="M1066">
         <v>0</v>
       </c>
@@ -21467,6 +21522,13 @@
       <c r="D1073">
         <v>1421.1</v>
       </c>
+      <c r="G1073">
+        <f>H1073*U1073</f>
+        <v>0.18239239999999998</v>
+      </c>
+      <c r="H1073" s="3">
+        <v>30.4</v>
+      </c>
       <c r="L1073">
         <v>1.4817500000000001E-2</v>
       </c>
@@ -21623,6 +21685,13 @@
       <c r="D1076">
         <v>1779.9</v>
       </c>
+      <c r="G1076">
+        <f>H1076*U1076</f>
+        <v>0.18212414999999998</v>
+      </c>
+      <c r="H1076" s="3">
+        <v>35.4</v>
+      </c>
       <c r="L1076">
         <v>9.4787499999999993E-3</v>
       </c>
@@ -22027,6 +22096,13 @@
       <c r="D1092">
         <v>56.2</v>
       </c>
+      <c r="G1092">
+        <f>H1092*U1092</f>
+        <v>0</v>
+      </c>
+      <c r="H1092" s="3">
+        <v>0</v>
+      </c>
       <c r="M1092">
         <v>0</v>
       </c>
@@ -22552,6 +22628,13 @@
       <c r="D1107">
         <v>543.5</v>
       </c>
+      <c r="G1107">
+        <f>H1107*U1107</f>
+        <v>0.23437419999999998</v>
+      </c>
+      <c r="H1107" s="3">
+        <v>48.8</v>
+      </c>
       <c r="M1107">
         <v>0</v>
       </c>
@@ -22791,6 +22874,13 @@
       <c r="D1114">
         <v>685.1</v>
       </c>
+      <c r="G1114">
+        <f>H1114*U1114</f>
+        <v>0.30068690000000003</v>
+      </c>
+      <c r="H1114" s="3">
+        <v>70.900000000000006</v>
+      </c>
       <c r="L1114">
         <v>1.45275E-2</v>
       </c>
@@ -22935,6 +23025,13 @@
       <c r="D1117">
         <v>795.4</v>
       </c>
+      <c r="G1117">
+        <f>H1117*U1117</f>
+        <v>0.30265229999999999</v>
+      </c>
+      <c r="H1117" s="3">
+        <v>70.8</v>
+      </c>
       <c r="L1117">
         <v>8.2565E-3</v>
       </c>
@@ -23339,6 +23436,13 @@
       <c r="D1133">
         <v>58.05</v>
       </c>
+      <c r="G1133">
+        <f>H1133*U1133</f>
+        <v>0</v>
+      </c>
+      <c r="H1133" s="3">
+        <v>0</v>
+      </c>
       <c r="M1133">
         <v>0</v>
       </c>
@@ -23840,6 +23944,13 @@
       <c r="D1148">
         <v>1100</v>
       </c>
+      <c r="G1148">
+        <f>H1148*U1148</f>
+        <v>9.2931299999999994E-2</v>
+      </c>
+      <c r="H1148" s="3">
+        <v>15.4</v>
+      </c>
       <c r="M1148">
         <v>0</v>
       </c>
@@ -24079,6 +24190,13 @@
       <c r="D1155">
         <v>1886</v>
       </c>
+      <c r="G1155">
+        <f>H1155*U1155</f>
+        <v>0.15641677499999998</v>
+      </c>
+      <c r="H1155" s="3">
+        <v>26.9</v>
+      </c>
       <c r="L1155">
         <v>1.57225E-2</v>
       </c>
@@ -24223,6 +24341,13 @@
       <c r="D1158">
         <v>2445.9299999999998</v>
       </c>
+      <c r="G1158">
+        <f>H1158*U1158</f>
+        <v>0.15839745</v>
+      </c>
+      <c r="H1158" s="3">
+        <v>27.8</v>
+      </c>
       <c r="L1158">
         <v>1.0737500000000001E-2</v>
       </c>
@@ -24627,6 +24752,13 @@
       <c r="D1174">
         <v>71.900000000000006</v>
       </c>
+      <c r="G1174">
+        <f>H1174*U1174</f>
+        <v>0</v>
+      </c>
+      <c r="H1174" s="3">
+        <v>0</v>
+      </c>
       <c r="M1174">
         <v>0</v>
       </c>
@@ -25140,6 +25272,13 @@
       <c r="D1189">
         <v>640.1</v>
       </c>
+      <c r="G1189">
+        <f>H1189*U1189</f>
+        <v>0.2056306</v>
+      </c>
+      <c r="H1189" s="3">
+        <v>38.200000000000003</v>
+      </c>
       <c r="M1189">
         <v>0</v>
       </c>
@@ -25379,6 +25518,13 @@
       <c r="D1196">
         <v>918.3</v>
       </c>
+      <c r="G1196">
+        <f>H1196*U1196</f>
+        <v>0.29001885000000005</v>
+      </c>
+      <c r="H1196" s="3">
+        <v>62.7</v>
+      </c>
       <c r="L1196">
         <v>1.4907500000000001E-2</v>
       </c>
@@ -25523,6 +25669,13 @@
       <c r="D1199">
         <v>1045.8800000000001</v>
       </c>
+      <c r="G1199">
+        <f>H1199*U1199</f>
+        <v>0.49520269999999994</v>
+      </c>
+      <c r="H1199" s="3">
+        <v>99.1</v>
+      </c>
       <c r="L1199">
         <v>9.9885000000000009E-3</v>
       </c>
@@ -25927,6 +26080,13 @@
       <c r="D1215">
         <v>67.5</v>
       </c>
+      <c r="G1215">
+        <f>H1215*U1215</f>
+        <v>0</v>
+      </c>
+      <c r="H1215" s="3">
+        <v>0</v>
+      </c>
       <c r="M1215">
         <v>0</v>
       </c>
@@ -26416,6 +26576,13 @@
       <c r="D1230">
         <v>1256.8</v>
       </c>
+      <c r="G1230">
+        <f>H1230*U1230</f>
+        <v>6.0058663999999998E-2</v>
+      </c>
+      <c r="H1230" s="3">
+        <v>8</v>
+      </c>
       <c r="M1230">
         <v>0</v>
       </c>
@@ -26655,6 +26822,13 @@
       <c r="D1237">
         <v>2181.3000000000002</v>
       </c>
+      <c r="G1237">
+        <f>H1237*U1237</f>
+        <v>7.895474999999999E-2</v>
+      </c>
+      <c r="H1237" s="3">
+        <v>8.1</v>
+      </c>
       <c r="L1237">
         <v>1.9025E-2</v>
       </c>
@@ -26799,6 +26973,13 @@
       <c r="D1240">
         <v>2695.5</v>
       </c>
+      <c r="G1240">
+        <f>H1240*U1240</f>
+        <v>2.77389E-2</v>
+      </c>
+      <c r="H1240" s="3">
+        <v>5.0999999999999996</v>
+      </c>
       <c r="L1240">
         <v>1.2607500000000001E-2</v>
       </c>
@@ -27203,6 +27384,13 @@
       <c r="D1256">
         <v>68.349999999999994</v>
       </c>
+      <c r="G1256">
+        <f>H1256*U1256</f>
+        <v>0</v>
+      </c>
+      <c r="H1256" s="3">
+        <v>0</v>
+      </c>
       <c r="M1256">
         <v>0</v>
       </c>
@@ -27704,6 +27892,13 @@
       <c r="D1271">
         <v>756.8</v>
       </c>
+      <c r="G1271">
+        <f>H1271*U1271</f>
+        <v>0.28058135000000001</v>
+      </c>
+      <c r="H1271" s="3">
+        <v>49.7</v>
+      </c>
       <c r="M1271">
         <v>0</v>
       </c>
@@ -27943,6 +28138,13 @@
       <c r="D1278">
         <v>982.9</v>
       </c>
+      <c r="G1278">
+        <f>H1278*U1278</f>
+        <v>0.32830417499999992</v>
+      </c>
+      <c r="H1278" s="3">
+        <v>64.099999999999994</v>
+      </c>
       <c r="L1278">
         <v>1.5727499999999998E-2</v>
       </c>
@@ -28086,6 +28288,13 @@
       </c>
       <c r="D1281">
         <v>1077.08</v>
+      </c>
+      <c r="G1281">
+        <f>H1281*U1281</f>
+        <v>0.35764750000000001</v>
+      </c>
+      <c r="H1281" s="3">
+        <v>76.400000000000006</v>
       </c>
       <c r="L1281">
         <v>9.3257500000000007E-3</v>

</xml_diff>

<commit_message>
Change variable name in observed files from Nconc to NConc
</commit_message>
<xml_diff>
--- a/Tests/Validation/Maize/Observations/MaizeObservations.xlsx
+++ b/Tests/Validation/Maize/Observations/MaizeObservations.xlsx
@@ -742,9 +742,6 @@
     <t>Maize.Stem.NConc</t>
   </si>
   <si>
-    <t>Maize.Spike.Nconc</t>
-  </si>
-  <si>
     <t>Maize.Spike.N</t>
   </si>
   <si>
@@ -758,6 +755,9 @@
   </si>
   <si>
     <t>NodesStartedSenescing</t>
+  </si>
+  <si>
+    <t>Maize.Spike.NConc</t>
   </si>
 </sst>
 </file>
@@ -1141,10 +1141,10 @@
   <dimension ref="A1:BU1635"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
-      <pane xSplit="2" ySplit="1" topLeftCell="BP74" activePane="bottomRight" state="frozen"/>
+      <pane xSplit="2" ySplit="1" topLeftCell="AC2" activePane="bottomRight" state="frozen"/>
       <selection pane="topRight" activeCell="C1" sqref="C1"/>
       <selection pane="bottomLeft" activeCell="A2" sqref="A2"/>
-      <selection pane="bottomRight" activeCell="BU74" sqref="BU74"/>
+      <selection pane="bottomRight" activeCell="AI74" sqref="AI74"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -1254,13 +1254,13 @@
         <v>235</v>
       </c>
       <c r="AH1" t="s">
+        <v>239</v>
+      </c>
+      <c r="AI1" t="s">
+        <v>244</v>
+      </c>
+      <c r="AJ1" t="s">
         <v>240</v>
-      </c>
-      <c r="AI1" t="s">
-        <v>239</v>
-      </c>
-      <c r="AJ1" t="s">
-        <v>241</v>
       </c>
       <c r="AK1" s="2" t="s">
         <v>230</v>
@@ -1365,13 +1365,13 @@
         <v>3</v>
       </c>
       <c r="BS1" s="1" t="s">
+        <v>241</v>
+      </c>
+      <c r="BT1" s="1" t="s">
         <v>242</v>
       </c>
-      <c r="BT1" s="1" t="s">
+      <c r="BU1" s="1" t="s">
         <v>243</v>
-      </c>
-      <c r="BU1" s="1" t="s">
-        <v>244</v>
       </c>
     </row>
     <row r="2" spans="1:73" hidden="1" x14ac:dyDescent="0.25">

</xml_diff>

<commit_message>
Fix problem with data
</commit_message>
<xml_diff>
--- a/Tests/Validation/Maize/Observations/MaizeObservations.xlsx
+++ b/Tests/Validation/Maize/Observations/MaizeObservations.xlsx
@@ -23,7 +23,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="2342" uniqueCount="247">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="2344" uniqueCount="247">
   <si>
     <t>AreaLargestLeaf</t>
   </si>
@@ -1146,10 +1146,10 @@
   <dimension ref="A1:BU1649"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
-      <pane xSplit="2" ySplit="1" topLeftCell="C1630" activePane="bottomRight" state="frozen"/>
+      <pane xSplit="2" ySplit="1" topLeftCell="Z1633" activePane="bottomRight" state="frozen"/>
       <selection pane="topRight" activeCell="C1" sqref="C1"/>
       <selection pane="bottomLeft" activeCell="A2" sqref="A2"/>
-      <selection pane="bottomRight" activeCell="G1633" sqref="G1633"/>
+      <selection pane="bottomRight" activeCell="AC1650" sqref="AC1650"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -41141,6 +41141,9 @@
       <c r="Z1641">
         <v>0</v>
       </c>
+      <c r="AC1641" t="s">
+        <v>202</v>
+      </c>
       <c r="AK1641">
         <v>6.2259565989999999</v>
       </c>
@@ -41522,6 +41525,9 @@
       </c>
       <c r="Z1649">
         <v>0</v>
+      </c>
+      <c r="AC1649" t="s">
+        <v>202</v>
       </c>
       <c r="AK1649">
         <v>5.4365841970000002</v>

</xml_diff>

<commit_message>
End Day one of sprint
</commit_message>
<xml_diff>
--- a/Tests/Validation/Maize/Observations/MaizeObservations.xlsx
+++ b/Tests/Validation/Maize/Observations/MaizeObservations.xlsx
@@ -8,7 +8,7 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Work\Repos\APSIMX\Tests\Validation\Maize\Observations\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{8F026255-F864-4F5B-A7E6-DC30CF17D577}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{361F2ED1-6012-42DC-8753-1AC2A4B67DAD}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
     <workbookView xWindow="-98" yWindow="-98" windowWidth="20715" windowHeight="13155" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
@@ -568,9 +568,6 @@
     <t>Maize.Leaf.Dead.Wt</t>
   </si>
   <si>
-    <t>Maize.Structure.FinalLeafNumber</t>
-  </si>
-  <si>
     <t>Maize.Grain.N</t>
   </si>
   <si>
@@ -770,6 +767,9 @@
   </si>
   <si>
     <t>Maize.Leaf.Tips</t>
+  </si>
+  <si>
+    <t>Maize.Leaf.FinalLeafNumber</t>
   </si>
 </sst>
 </file>
@@ -1186,10 +1186,10 @@
   <dimension ref="A1:BU1635"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
-      <pane xSplit="2" ySplit="1" topLeftCell="P2" activePane="bottomRight" state="frozen"/>
+      <pane xSplit="2" ySplit="1" topLeftCell="AD54" activePane="bottomRight" state="frozen"/>
       <selection pane="topRight" activeCell="C1" sqref="C1"/>
       <selection pane="bottomLeft" activeCell="A2" sqref="A2"/>
-      <selection pane="bottomRight" activeCell="P2" sqref="P2"/>
+      <selection pane="bottomRight" activeCell="AN80" sqref="AN80"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="14.25" x14ac:dyDescent="0.45"/>
@@ -1221,10 +1221,10 @@
         <v>6</v>
       </c>
       <c r="H1" t="s">
-        <v>194</v>
+        <v>193</v>
       </c>
       <c r="I1" t="s">
-        <v>178</v>
+        <v>177</v>
       </c>
       <c r="J1" t="s">
         <v>173</v>
@@ -1236,25 +1236,25 @@
         <v>174</v>
       </c>
       <c r="M1" t="s">
+        <v>188</v>
+      </c>
+      <c r="N1" t="s">
         <v>189</v>
       </c>
-      <c r="N1" t="s">
+      <c r="O1" t="s">
         <v>190</v>
       </c>
-      <c r="O1" t="s">
-        <v>191</v>
-      </c>
       <c r="P1" t="s">
-        <v>244</v>
+        <v>243</v>
       </c>
       <c r="Q1" t="s">
-        <v>179</v>
+        <v>178</v>
       </c>
       <c r="R1" t="s">
         <v>175</v>
       </c>
       <c r="S1" t="s">
-        <v>180</v>
+        <v>179</v>
       </c>
       <c r="T1" t="s">
         <v>176</v>
@@ -1263,7 +1263,7 @@
         <v>7</v>
       </c>
       <c r="V1" t="s">
-        <v>243</v>
+        <v>242</v>
       </c>
       <c r="W1" t="s">
         <v>8</v>
@@ -1272,52 +1272,52 @@
         <v>9</v>
       </c>
       <c r="Y1" t="s">
+        <v>180</v>
+      </c>
+      <c r="Z1" t="s">
         <v>181</v>
       </c>
-      <c r="Z1" t="s">
+      <c r="AA1" t="s">
         <v>182</v>
       </c>
-      <c r="AA1" t="s">
+      <c r="AB1" t="s">
         <v>183</v>
       </c>
-      <c r="AB1" t="s">
+      <c r="AC1" t="s">
         <v>184</v>
       </c>
-      <c r="AC1" t="s">
+      <c r="AD1" t="s">
+        <v>186</v>
+      </c>
+      <c r="AE1" s="2" t="s">
+        <v>191</v>
+      </c>
+      <c r="AF1" t="s">
+        <v>194</v>
+      </c>
+      <c r="AG1" t="s">
+        <v>192</v>
+      </c>
+      <c r="AH1" t="s">
+        <v>196</v>
+      </c>
+      <c r="AI1" t="s">
+        <v>201</v>
+      </c>
+      <c r="AJ1" t="s">
+        <v>197</v>
+      </c>
+      <c r="AK1" s="2" t="s">
+        <v>187</v>
+      </c>
+      <c r="AL1" t="s">
+        <v>195</v>
+      </c>
+      <c r="AM1" t="s">
         <v>185</v>
       </c>
-      <c r="AD1" t="s">
-        <v>187</v>
-      </c>
-      <c r="AE1" s="2" t="s">
-        <v>192</v>
-      </c>
-      <c r="AF1" t="s">
-        <v>195</v>
-      </c>
-      <c r="AG1" t="s">
-        <v>193</v>
-      </c>
-      <c r="AH1" t="s">
-        <v>197</v>
-      </c>
-      <c r="AI1" t="s">
-        <v>202</v>
-      </c>
-      <c r="AJ1" t="s">
-        <v>198</v>
-      </c>
-      <c r="AK1" s="2" t="s">
-        <v>188</v>
-      </c>
-      <c r="AL1" t="s">
-        <v>196</v>
-      </c>
-      <c r="AM1" t="s">
-        <v>186</v>
-      </c>
       <c r="AN1" t="s">
-        <v>177</v>
+        <v>244</v>
       </c>
       <c r="AO1" t="s">
         <v>10</v>
@@ -1332,52 +1332,52 @@
         <v>13</v>
       </c>
       <c r="AS1" t="s">
+        <v>226</v>
+      </c>
+      <c r="AT1" t="s">
         <v>227</v>
       </c>
-      <c r="AT1" t="s">
+      <c r="AU1" t="s">
         <v>228</v>
       </c>
-      <c r="AU1" t="s">
+      <c r="AV1" t="s">
         <v>229</v>
       </c>
-      <c r="AV1" t="s">
+      <c r="AW1" t="s">
         <v>230</v>
       </c>
-      <c r="AW1" t="s">
+      <c r="AX1" t="s">
         <v>231</v>
       </c>
-      <c r="AX1" t="s">
+      <c r="AY1" t="s">
         <v>232</v>
       </c>
-      <c r="AY1" t="s">
+      <c r="AZ1" t="s">
         <v>233</v>
       </c>
-      <c r="AZ1" t="s">
+      <c r="BA1" t="s">
         <v>234</v>
       </c>
-      <c r="BA1" t="s">
+      <c r="BB1" t="s">
         <v>235</v>
       </c>
-      <c r="BB1" t="s">
+      <c r="BC1" t="s">
         <v>236</v>
       </c>
-      <c r="BC1" t="s">
+      <c r="BD1" t="s">
         <v>237</v>
       </c>
-      <c r="BD1" t="s">
+      <c r="BE1" t="s">
         <v>238</v>
       </c>
-      <c r="BE1" t="s">
+      <c r="BF1" t="s">
         <v>239</v>
       </c>
-      <c r="BF1" t="s">
+      <c r="BG1" t="s">
         <v>240</v>
       </c>
-      <c r="BG1" t="s">
+      <c r="BH1" t="s">
         <v>241</v>
-      </c>
-      <c r="BH1" t="s">
-        <v>242</v>
       </c>
       <c r="BI1" t="s">
         <v>14</v>
@@ -1410,18 +1410,18 @@
         <v>3</v>
       </c>
       <c r="BS1" s="1" t="s">
+        <v>198</v>
+      </c>
+      <c r="BT1" s="1" t="s">
         <v>199</v>
       </c>
-      <c r="BT1" s="1" t="s">
+      <c r="BU1" s="1" t="s">
         <v>200</v>
-      </c>
-      <c r="BU1" s="1" t="s">
-        <v>201</v>
       </c>
     </row>
     <row r="2" spans="1:73" x14ac:dyDescent="0.45">
       <c r="A2" t="s">
-        <v>203</v>
+        <v>202</v>
       </c>
       <c r="B2" s="3">
         <v>73051</v>
@@ -1455,7 +1455,7 @@
     </row>
     <row r="3" spans="1:73" x14ac:dyDescent="0.45">
       <c r="A3" t="s">
-        <v>204</v>
+        <v>203</v>
       </c>
       <c r="B3" s="3">
         <v>73051</v>
@@ -1489,7 +1489,7 @@
     </row>
     <row r="4" spans="1:73" x14ac:dyDescent="0.45">
       <c r="A4" t="s">
-        <v>205</v>
+        <v>204</v>
       </c>
       <c r="B4" s="3">
         <v>73051</v>
@@ -1523,7 +1523,7 @@
     </row>
     <row r="5" spans="1:73" x14ac:dyDescent="0.45">
       <c r="A5" t="s">
-        <v>206</v>
+        <v>205</v>
       </c>
       <c r="B5" s="3">
         <v>73051</v>
@@ -1557,7 +1557,7 @@
     </row>
     <row r="6" spans="1:73" x14ac:dyDescent="0.45">
       <c r="A6" t="s">
-        <v>207</v>
+        <v>206</v>
       </c>
       <c r="B6" s="3">
         <v>73051</v>
@@ -1591,7 +1591,7 @@
     </row>
     <row r="7" spans="1:73" x14ac:dyDescent="0.45">
       <c r="A7" t="s">
-        <v>208</v>
+        <v>207</v>
       </c>
       <c r="B7" s="3">
         <v>73051</v>
@@ -1625,7 +1625,7 @@
     </row>
     <row r="8" spans="1:73" x14ac:dyDescent="0.45">
       <c r="A8" t="s">
-        <v>209</v>
+        <v>208</v>
       </c>
       <c r="B8" s="3">
         <v>73051</v>
@@ -1659,7 +1659,7 @@
     </row>
     <row r="9" spans="1:73" x14ac:dyDescent="0.45">
       <c r="A9" t="s">
-        <v>210</v>
+        <v>209</v>
       </c>
       <c r="B9" s="3">
         <v>73051</v>
@@ -1693,7 +1693,7 @@
     </row>
     <row r="10" spans="1:73" x14ac:dyDescent="0.45">
       <c r="A10" t="s">
-        <v>211</v>
+        <v>210</v>
       </c>
       <c r="B10" s="3">
         <v>73051</v>
@@ -1727,7 +1727,7 @@
     </row>
     <row r="11" spans="1:73" x14ac:dyDescent="0.45">
       <c r="A11" t="s">
-        <v>212</v>
+        <v>211</v>
       </c>
       <c r="B11" s="3">
         <v>73051</v>
@@ -1761,7 +1761,7 @@
     </row>
     <row r="12" spans="1:73" x14ac:dyDescent="0.45">
       <c r="A12" t="s">
-        <v>213</v>
+        <v>212</v>
       </c>
       <c r="B12" s="3">
         <v>73051</v>
@@ -1795,7 +1795,7 @@
     </row>
     <row r="13" spans="1:73" x14ac:dyDescent="0.45">
       <c r="A13" t="s">
-        <v>214</v>
+        <v>213</v>
       </c>
       <c r="B13" s="3">
         <v>73051</v>
@@ -1829,7 +1829,7 @@
     </row>
     <row r="14" spans="1:73" x14ac:dyDescent="0.45">
       <c r="A14" t="s">
-        <v>215</v>
+        <v>214</v>
       </c>
       <c r="B14" s="3">
         <v>73051</v>
@@ -1863,7 +1863,7 @@
     </row>
     <row r="15" spans="1:73" x14ac:dyDescent="0.45">
       <c r="A15" t="s">
-        <v>216</v>
+        <v>215</v>
       </c>
       <c r="B15" s="3">
         <v>73051</v>
@@ -1897,7 +1897,7 @@
     </row>
     <row r="16" spans="1:73" x14ac:dyDescent="0.45">
       <c r="A16" t="s">
-        <v>217</v>
+        <v>216</v>
       </c>
       <c r="B16" s="3">
         <v>73051</v>
@@ -1931,7 +1931,7 @@
     </row>
     <row r="17" spans="1:70" x14ac:dyDescent="0.45">
       <c r="A17" t="s">
-        <v>218</v>
+        <v>217</v>
       </c>
       <c r="B17" s="3">
         <v>73051</v>
@@ -1965,7 +1965,7 @@
     </row>
     <row r="18" spans="1:70" x14ac:dyDescent="0.45">
       <c r="A18" t="s">
-        <v>219</v>
+        <v>218</v>
       </c>
       <c r="B18" s="3">
         <v>73051</v>
@@ -1999,7 +1999,7 @@
     </row>
     <row r="19" spans="1:70" x14ac:dyDescent="0.45">
       <c r="A19" t="s">
-        <v>220</v>
+        <v>219</v>
       </c>
       <c r="B19" s="3">
         <v>73051</v>
@@ -2033,7 +2033,7 @@
     </row>
     <row r="20" spans="1:70" x14ac:dyDescent="0.45">
       <c r="A20" t="s">
-        <v>221</v>
+        <v>220</v>
       </c>
       <c r="B20" s="3">
         <v>73051</v>
@@ -2067,7 +2067,7 @@
     </row>
     <row r="21" spans="1:70" x14ac:dyDescent="0.45">
       <c r="A21" t="s">
-        <v>222</v>
+        <v>221</v>
       </c>
       <c r="B21" s="3">
         <v>73051</v>
@@ -2101,7 +2101,7 @@
     </row>
     <row r="22" spans="1:70" x14ac:dyDescent="0.45">
       <c r="A22" t="s">
-        <v>223</v>
+        <v>222</v>
       </c>
       <c r="B22" s="3">
         <v>73051</v>
@@ -2135,7 +2135,7 @@
     </row>
     <row r="23" spans="1:70" x14ac:dyDescent="0.45">
       <c r="A23" t="s">
-        <v>224</v>
+        <v>223</v>
       </c>
       <c r="B23" s="3">
         <v>73051</v>
@@ -2169,7 +2169,7 @@
     </row>
     <row r="24" spans="1:70" x14ac:dyDescent="0.45">
       <c r="A24" t="s">
-        <v>225</v>
+        <v>224</v>
       </c>
       <c r="B24" s="3">
         <v>73051</v>
@@ -2203,7 +2203,7 @@
     </row>
     <row r="25" spans="1:70" x14ac:dyDescent="0.45">
       <c r="A25" t="s">
-        <v>226</v>
+        <v>225</v>
       </c>
       <c r="B25" s="3">
         <v>73051</v>

</xml_diff>

<commit_message>
Add a Phenology.CurrentStageName to data for new sims.
</commit_message>
<xml_diff>
--- a/Tests/Validation/Maize/Observations/MaizeObservations.xlsx
+++ b/Tests/Validation/Maize/Observations/MaizeObservations.xlsx
@@ -8,7 +8,7 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\ilhuber\NextGen\ApsimX\Tests\Validation\Maize\Observations\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{3998A2DB-BF50-4B40-AEC7-2CC179D1EF51}" xr6:coauthVersionLast="36" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{07EF50CA-A154-4CB9-BB8F-5F5281AC086C}" xr6:coauthVersionLast="36" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
     <workbookView xWindow="1905" yWindow="1185" windowWidth="21915" windowHeight="13215" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
@@ -35,7 +35,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="2378" uniqueCount="297">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="2430" uniqueCount="297">
   <si>
     <t>AreaLargestLeaf</t>
   </si>
@@ -1342,10 +1342,10 @@
   <dimension ref="A1:BU1685"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
-      <pane xSplit="2" ySplit="1" topLeftCell="C1700" activePane="bottomRight" state="frozen"/>
+      <pane xSplit="2" ySplit="1" topLeftCell="L1597" activePane="bottomRight" state="frozen"/>
       <selection pane="topRight" activeCell="C1" sqref="C1"/>
       <selection pane="bottomLeft" activeCell="A2" sqref="A2"/>
-      <selection pane="bottomRight" activeCell="J1678" sqref="J1678"/>
+      <selection pane="bottomRight" activeCell="AC1634" sqref="AC1634"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -40986,6 +40986,9 @@
       <c r="L1634">
         <v>1240.71</v>
       </c>
+      <c r="AC1634" t="s">
+        <v>162</v>
+      </c>
     </row>
     <row r="1635" spans="1:68" x14ac:dyDescent="0.25">
       <c r="A1635" t="s">
@@ -41003,6 +41006,9 @@
       <c r="L1635">
         <v>909.7700000000001</v>
       </c>
+      <c r="AC1635" t="s">
+        <v>162</v>
+      </c>
       <c r="AJ1635">
         <v>0.7</v>
       </c>
@@ -41023,6 +41029,9 @@
       <c r="L1636">
         <v>671.6</v>
       </c>
+      <c r="AC1636" t="s">
+        <v>162</v>
+      </c>
     </row>
     <row r="1637" spans="1:68" x14ac:dyDescent="0.25">
       <c r="A1637" t="s">
@@ -41040,6 +41049,9 @@
       <c r="L1637">
         <v>436.53999999999996</v>
       </c>
+      <c r="AC1637" t="s">
+        <v>162</v>
+      </c>
     </row>
     <row r="1638" spans="1:68" x14ac:dyDescent="0.25">
       <c r="A1638" t="s">
@@ -41057,6 +41069,9 @@
       <c r="L1638">
         <v>1166.27</v>
       </c>
+      <c r="AC1638" t="s">
+        <v>162</v>
+      </c>
     </row>
     <row r="1639" spans="1:68" x14ac:dyDescent="0.25">
       <c r="A1639" t="s">
@@ -41074,6 +41089,9 @@
       <c r="L1639">
         <v>856.82</v>
       </c>
+      <c r="AC1639" t="s">
+        <v>162</v>
+      </c>
     </row>
     <row r="1640" spans="1:68" x14ac:dyDescent="0.25">
       <c r="A1640" t="s">
@@ -41091,6 +41109,9 @@
       <c r="L1640">
         <v>597.15</v>
       </c>
+      <c r="AC1640" t="s">
+        <v>162</v>
+      </c>
     </row>
     <row r="1641" spans="1:68" x14ac:dyDescent="0.25">
       <c r="A1641" t="s">
@@ -41108,6 +41129,9 @@
       <c r="L1641">
         <v>1184.46</v>
       </c>
+      <c r="AC1641" t="s">
+        <v>162</v>
+      </c>
     </row>
     <row r="1642" spans="1:68" x14ac:dyDescent="0.25">
       <c r="A1642" t="s">
@@ -41125,6 +41149,9 @@
       <c r="L1642">
         <v>1132.6299999999999</v>
       </c>
+      <c r="AC1642" t="s">
+        <v>162</v>
+      </c>
     </row>
     <row r="1643" spans="1:68" x14ac:dyDescent="0.25">
       <c r="A1643" t="s">
@@ -41142,6 +41169,9 @@
       <c r="L1643">
         <v>964.45</v>
       </c>
+      <c r="AC1643" t="s">
+        <v>162</v>
+      </c>
     </row>
     <row r="1644" spans="1:68" x14ac:dyDescent="0.25">
       <c r="A1644" t="s">
@@ -41159,6 +41189,9 @@
       <c r="L1644">
         <v>973.11</v>
       </c>
+      <c r="AC1644" t="s">
+        <v>162</v>
+      </c>
     </row>
     <row r="1645" spans="1:68" x14ac:dyDescent="0.25">
       <c r="A1645" t="s">
@@ -41176,6 +41209,9 @@
       <c r="L1645">
         <v>674.53</v>
       </c>
+      <c r="AC1645" t="s">
+        <v>162</v>
+      </c>
     </row>
     <row r="1646" spans="1:68" x14ac:dyDescent="0.25">
       <c r="A1646" t="s">
@@ -41193,6 +41229,9 @@
       <c r="L1646">
         <v>477.18999999999994</v>
       </c>
+      <c r="AC1646" t="s">
+        <v>162</v>
+      </c>
     </row>
     <row r="1647" spans="1:68" x14ac:dyDescent="0.25">
       <c r="A1647" t="s">
@@ -41210,6 +41249,9 @@
       <c r="L1647">
         <v>1184.7</v>
       </c>
+      <c r="AC1647" t="s">
+        <v>162</v>
+      </c>
     </row>
     <row r="1648" spans="1:68" x14ac:dyDescent="0.25">
       <c r="A1648" t="s">
@@ -41227,8 +41269,11 @@
       <c r="L1648">
         <v>884.07999999999993</v>
       </c>
-    </row>
-    <row r="1649" spans="1:12" x14ac:dyDescent="0.25">
+      <c r="AC1648" t="s">
+        <v>162</v>
+      </c>
+    </row>
+    <row r="1649" spans="1:29" x14ac:dyDescent="0.25">
       <c r="A1649" t="s">
         <v>260</v>
       </c>
@@ -41244,8 +41289,11 @@
       <c r="L1649">
         <v>647.75</v>
       </c>
-    </row>
-    <row r="1650" spans="1:12" x14ac:dyDescent="0.25">
+      <c r="AC1649" t="s">
+        <v>162</v>
+      </c>
+    </row>
+    <row r="1650" spans="1:29" x14ac:dyDescent="0.25">
       <c r="A1650" t="s">
         <v>261</v>
       </c>
@@ -41261,8 +41309,11 @@
       <c r="L1650">
         <v>1182.94</v>
       </c>
-    </row>
-    <row r="1651" spans="1:12" x14ac:dyDescent="0.25">
+      <c r="AC1650" t="s">
+        <v>162</v>
+      </c>
+    </row>
+    <row r="1651" spans="1:29" x14ac:dyDescent="0.25">
       <c r="A1651" t="s">
         <v>262</v>
       </c>
@@ -41278,8 +41329,11 @@
       <c r="L1651">
         <v>1138.6600000000001</v>
       </c>
-    </row>
-    <row r="1652" spans="1:12" x14ac:dyDescent="0.25">
+      <c r="AC1651" t="s">
+        <v>162</v>
+      </c>
+    </row>
+    <row r="1652" spans="1:29" x14ac:dyDescent="0.25">
       <c r="A1652" t="s">
         <v>263</v>
       </c>
@@ -41295,8 +41349,11 @@
       <c r="L1652">
         <v>952.68999999999994</v>
       </c>
-    </row>
-    <row r="1653" spans="1:12" x14ac:dyDescent="0.25">
+      <c r="AC1652" t="s">
+        <v>162</v>
+      </c>
+    </row>
+    <row r="1653" spans="1:29" x14ac:dyDescent="0.25">
       <c r="A1653" t="s">
         <v>264</v>
       </c>
@@ -41312,8 +41369,11 @@
       <c r="L1653">
         <v>1174.1100000000001</v>
       </c>
-    </row>
-    <row r="1654" spans="1:12" x14ac:dyDescent="0.25">
+      <c r="AC1653" t="s">
+        <v>162</v>
+      </c>
+    </row>
+    <row r="1654" spans="1:29" x14ac:dyDescent="0.25">
       <c r="A1654" t="s">
         <v>265</v>
       </c>
@@ -41329,8 +41389,11 @@
       <c r="L1654">
         <v>878.43999999999994</v>
       </c>
-    </row>
-    <row r="1655" spans="1:12" x14ac:dyDescent="0.25">
+      <c r="AC1654" t="s">
+        <v>162</v>
+      </c>
+    </row>
+    <row r="1655" spans="1:29" x14ac:dyDescent="0.25">
       <c r="A1655" t="s">
         <v>266</v>
       </c>
@@ -41346,8 +41409,11 @@
       <c r="L1655">
         <v>652.04</v>
       </c>
-    </row>
-    <row r="1656" spans="1:12" x14ac:dyDescent="0.25">
+      <c r="AC1655" t="s">
+        <v>162</v>
+      </c>
+    </row>
+    <row r="1656" spans="1:29" x14ac:dyDescent="0.25">
       <c r="A1656" t="s">
         <v>267</v>
       </c>
@@ -41363,8 +41429,11 @@
       <c r="L1656">
         <v>461.82</v>
       </c>
-    </row>
-    <row r="1657" spans="1:12" x14ac:dyDescent="0.25">
+      <c r="AC1656" t="s">
+        <v>162</v>
+      </c>
+    </row>
+    <row r="1657" spans="1:29" x14ac:dyDescent="0.25">
       <c r="A1657" t="s">
         <v>268</v>
       </c>
@@ -41380,8 +41449,11 @@
       <c r="L1657">
         <v>1062.3899999999999</v>
       </c>
-    </row>
-    <row r="1658" spans="1:12" x14ac:dyDescent="0.25">
+      <c r="AC1657" t="s">
+        <v>162</v>
+      </c>
+    </row>
+    <row r="1658" spans="1:29" x14ac:dyDescent="0.25">
       <c r="A1658" t="s">
         <v>269</v>
       </c>
@@ -41397,8 +41469,11 @@
       <c r="L1658">
         <v>867.46</v>
       </c>
-    </row>
-    <row r="1659" spans="1:12" x14ac:dyDescent="0.25">
+      <c r="AC1658" t="s">
+        <v>162</v>
+      </c>
+    </row>
+    <row r="1659" spans="1:29" x14ac:dyDescent="0.25">
       <c r="A1659" t="s">
         <v>270</v>
       </c>
@@ -41414,8 +41489,11 @@
       <c r="L1659">
         <v>639.43999999999994</v>
       </c>
-    </row>
-    <row r="1660" spans="1:12" x14ac:dyDescent="0.25">
+      <c r="AC1659" t="s">
+        <v>162</v>
+      </c>
+    </row>
+    <row r="1660" spans="1:29" x14ac:dyDescent="0.25">
       <c r="A1660" t="s">
         <v>271</v>
       </c>
@@ -41431,8 +41509,11 @@
       <c r="L1660">
         <v>1140.75</v>
       </c>
-    </row>
-    <row r="1661" spans="1:12" x14ac:dyDescent="0.25">
+      <c r="AC1660" t="s">
+        <v>162</v>
+      </c>
+    </row>
+    <row r="1661" spans="1:29" x14ac:dyDescent="0.25">
       <c r="A1661" t="s">
         <v>272</v>
       </c>
@@ -41448,8 +41529,11 @@
       <c r="L1661">
         <v>1072.3200000000002</v>
       </c>
-    </row>
-    <row r="1662" spans="1:12" x14ac:dyDescent="0.25">
+      <c r="AC1661" t="s">
+        <v>162</v>
+      </c>
+    </row>
+    <row r="1662" spans="1:29" x14ac:dyDescent="0.25">
       <c r="A1662" t="s">
         <v>273</v>
       </c>
@@ -41465,8 +41549,11 @@
       <c r="L1662">
         <v>953.32</v>
       </c>
-    </row>
-    <row r="1663" spans="1:12" x14ac:dyDescent="0.25">
+      <c r="AC1662" t="s">
+        <v>162</v>
+      </c>
+    </row>
+    <row r="1663" spans="1:29" x14ac:dyDescent="0.25">
       <c r="A1663" t="s">
         <v>274</v>
       </c>
@@ -41482,8 +41569,11 @@
       <c r="L1663">
         <v>951.08999999999992</v>
       </c>
-    </row>
-    <row r="1664" spans="1:12" x14ac:dyDescent="0.25">
+      <c r="AC1663" t="s">
+        <v>162</v>
+      </c>
+    </row>
+    <row r="1664" spans="1:29" x14ac:dyDescent="0.25">
       <c r="A1664" t="s">
         <v>275</v>
       </c>
@@ -41499,8 +41589,11 @@
       <c r="L1664">
         <v>619.25</v>
       </c>
-    </row>
-    <row r="1665" spans="1:12" x14ac:dyDescent="0.25">
+      <c r="AC1664" t="s">
+        <v>162</v>
+      </c>
+    </row>
+    <row r="1665" spans="1:29" x14ac:dyDescent="0.25">
       <c r="A1665" t="s">
         <v>276</v>
       </c>
@@ -41516,8 +41609,11 @@
       <c r="L1665">
         <v>456.18999999999994</v>
       </c>
-    </row>
-    <row r="1666" spans="1:12" x14ac:dyDescent="0.25">
+      <c r="AC1665" t="s">
+        <v>162</v>
+      </c>
+    </row>
+    <row r="1666" spans="1:29" x14ac:dyDescent="0.25">
       <c r="A1666" t="s">
         <v>277</v>
       </c>
@@ -41533,8 +41629,11 @@
       <c r="L1666">
         <v>1076.6600000000001</v>
       </c>
-    </row>
-    <row r="1667" spans="1:12" x14ac:dyDescent="0.25">
+      <c r="AC1666" t="s">
+        <v>162</v>
+      </c>
+    </row>
+    <row r="1667" spans="1:29" x14ac:dyDescent="0.25">
       <c r="A1667" t="s">
         <v>278</v>
       </c>
@@ -41550,8 +41649,11 @@
       <c r="L1667">
         <v>845.92000000000007</v>
       </c>
-    </row>
-    <row r="1668" spans="1:12" x14ac:dyDescent="0.25">
+      <c r="AC1667" t="s">
+        <v>162</v>
+      </c>
+    </row>
+    <row r="1668" spans="1:29" x14ac:dyDescent="0.25">
       <c r="A1668" t="s">
         <v>279</v>
       </c>
@@ -41567,8 +41669,11 @@
       <c r="L1668">
         <v>633.28</v>
       </c>
-    </row>
-    <row r="1669" spans="1:12" x14ac:dyDescent="0.25">
+      <c r="AC1668" t="s">
+        <v>162</v>
+      </c>
+    </row>
+    <row r="1669" spans="1:29" x14ac:dyDescent="0.25">
       <c r="A1669" t="s">
         <v>280</v>
       </c>
@@ -41584,8 +41689,11 @@
       <c r="L1669">
         <v>1129.17</v>
       </c>
-    </row>
-    <row r="1670" spans="1:12" x14ac:dyDescent="0.25">
+      <c r="AC1669" t="s">
+        <v>162</v>
+      </c>
+    </row>
+    <row r="1670" spans="1:29" x14ac:dyDescent="0.25">
       <c r="A1670" t="s">
         <v>281</v>
       </c>
@@ -41601,8 +41709,11 @@
       <c r="L1670">
         <v>1079.54</v>
       </c>
-    </row>
-    <row r="1671" spans="1:12" x14ac:dyDescent="0.25">
+      <c r="AC1670" t="s">
+        <v>162</v>
+      </c>
+    </row>
+    <row r="1671" spans="1:29" x14ac:dyDescent="0.25">
       <c r="A1671" t="s">
         <v>282</v>
       </c>
@@ -41618,8 +41729,11 @@
       <c r="L1671">
         <v>947.42000000000007</v>
       </c>
-    </row>
-    <row r="1672" spans="1:12" x14ac:dyDescent="0.25">
+      <c r="AC1671" t="s">
+        <v>162</v>
+      </c>
+    </row>
+    <row r="1672" spans="1:29" x14ac:dyDescent="0.25">
       <c r="A1672" t="s">
         <v>283</v>
       </c>
@@ -41629,8 +41743,11 @@
       <c r="L1672">
         <v>970</v>
       </c>
-    </row>
-    <row r="1673" spans="1:12" x14ac:dyDescent="0.25">
+      <c r="AC1672" t="s">
+        <v>162</v>
+      </c>
+    </row>
+    <row r="1673" spans="1:29" x14ac:dyDescent="0.25">
       <c r="A1673" t="s">
         <v>284</v>
       </c>
@@ -41640,8 +41757,11 @@
       <c r="L1673">
         <v>955</v>
       </c>
-    </row>
-    <row r="1674" spans="1:12" x14ac:dyDescent="0.25">
+      <c r="AC1673" t="s">
+        <v>162</v>
+      </c>
+    </row>
+    <row r="1674" spans="1:29" x14ac:dyDescent="0.25">
       <c r="A1674" t="s">
         <v>285</v>
       </c>
@@ -41651,8 +41771,11 @@
       <c r="L1674">
         <v>872</v>
       </c>
-    </row>
-    <row r="1675" spans="1:12" x14ac:dyDescent="0.25">
+      <c r="AC1674" t="s">
+        <v>162</v>
+      </c>
+    </row>
+    <row r="1675" spans="1:29" x14ac:dyDescent="0.25">
       <c r="A1675" t="s">
         <v>286</v>
       </c>
@@ -41662,8 +41785,11 @@
       <c r="L1675">
         <v>690</v>
       </c>
-    </row>
-    <row r="1676" spans="1:12" x14ac:dyDescent="0.25">
+      <c r="AC1675" t="s">
+        <v>162</v>
+      </c>
+    </row>
+    <row r="1676" spans="1:29" x14ac:dyDescent="0.25">
       <c r="A1676" t="s">
         <v>287</v>
       </c>
@@ -41673,8 +41799,11 @@
       <c r="L1676">
         <v>1436</v>
       </c>
-    </row>
-    <row r="1677" spans="1:12" x14ac:dyDescent="0.25">
+      <c r="AC1676" t="s">
+        <v>162</v>
+      </c>
+    </row>
+    <row r="1677" spans="1:29" x14ac:dyDescent="0.25">
       <c r="A1677" t="s">
         <v>288</v>
       </c>
@@ -41684,8 +41813,11 @@
       <c r="L1677">
         <v>1319</v>
       </c>
-    </row>
-    <row r="1678" spans="1:12" x14ac:dyDescent="0.25">
+      <c r="AC1677" t="s">
+        <v>162</v>
+      </c>
+    </row>
+    <row r="1678" spans="1:29" x14ac:dyDescent="0.25">
       <c r="A1678" t="s">
         <v>289</v>
       </c>
@@ -41695,8 +41827,11 @@
       <c r="L1678">
         <v>1137</v>
       </c>
-    </row>
-    <row r="1679" spans="1:12" x14ac:dyDescent="0.25">
+      <c r="AC1678" t="s">
+        <v>162</v>
+      </c>
+    </row>
+    <row r="1679" spans="1:29" x14ac:dyDescent="0.25">
       <c r="A1679" t="s">
         <v>290</v>
       </c>
@@ -41706,8 +41841,11 @@
       <c r="L1679">
         <v>919</v>
       </c>
-    </row>
-    <row r="1680" spans="1:12" x14ac:dyDescent="0.25">
+      <c r="AC1679" t="s">
+        <v>162</v>
+      </c>
+    </row>
+    <row r="1680" spans="1:29" x14ac:dyDescent="0.25">
       <c r="A1680" t="s">
         <v>291</v>
       </c>
@@ -41717,8 +41855,11 @@
       <c r="L1680">
         <v>811.99999999999989</v>
       </c>
-    </row>
-    <row r="1681" spans="1:12" x14ac:dyDescent="0.25">
+      <c r="AC1680" t="s">
+        <v>162</v>
+      </c>
+    </row>
+    <row r="1681" spans="1:29" x14ac:dyDescent="0.25">
       <c r="A1681" t="s">
         <v>292</v>
       </c>
@@ -41728,8 +41869,11 @@
       <c r="L1681">
         <v>721</v>
       </c>
-    </row>
-    <row r="1682" spans="1:12" x14ac:dyDescent="0.25">
+      <c r="AC1681" t="s">
+        <v>162</v>
+      </c>
+    </row>
+    <row r="1682" spans="1:29" x14ac:dyDescent="0.25">
       <c r="A1682" t="s">
         <v>293</v>
       </c>
@@ -41739,8 +41883,11 @@
       <c r="L1682">
         <v>484</v>
       </c>
-    </row>
-    <row r="1683" spans="1:12" x14ac:dyDescent="0.25">
+      <c r="AC1682" t="s">
+        <v>162</v>
+      </c>
+    </row>
+    <row r="1683" spans="1:29" x14ac:dyDescent="0.25">
       <c r="A1683" t="s">
         <v>294</v>
       </c>
@@ -41750,8 +41897,11 @@
       <c r="L1683">
         <v>740</v>
       </c>
-    </row>
-    <row r="1684" spans="1:12" x14ac:dyDescent="0.25">
+      <c r="AC1683" t="s">
+        <v>162</v>
+      </c>
+    </row>
+    <row r="1684" spans="1:29" x14ac:dyDescent="0.25">
       <c r="A1684" t="s">
         <v>295</v>
       </c>
@@ -41761,8 +41911,11 @@
       <c r="L1684">
         <v>396</v>
       </c>
-    </row>
-    <row r="1685" spans="1:12" x14ac:dyDescent="0.25">
+      <c r="AC1684" t="s">
+        <v>162</v>
+      </c>
+    </row>
+    <row r="1685" spans="1:29" x14ac:dyDescent="0.25">
       <c r="A1685" t="s">
         <v>296</v>
       </c>
@@ -41771,6 +41924,9 @@
       </c>
       <c r="L1685">
         <v>432</v>
+      </c>
+      <c r="AC1685" t="s">
+        <v>162</v>
       </c>
     </row>
   </sheetData>

</xml_diff>